<commit_message>
Revert back to colorful odf
</commit_message>
<xml_diff>
--- a/resume_data.xlsx
+++ b/resume_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work project\vitae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A99A54-5FCB-46CC-8471-34ED7E5641DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4CFACF-DA55-4C23-8B86-4D05EB6E7586}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="positions" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="78">
   <si>
     <t>section</t>
   </si>
@@ -270,6 +270,27 @@
   </si>
   <si>
     <t>Web Scraping</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Worked on data analysis and visualisation, and bring data analytic techniques to bear on a wide variety of problems. Workedon tight (1-3 month) timeframes to deliver bespoke work on Data Analytics to clients.</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>development</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>CFA Level 1 Passed                                                                                                    Aug 2018 – Present</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFA Institute </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Present</t>
+  </si>
+  <si>
+    <t>Aug 2018</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -1140,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M152"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1284,7 +1305,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" ht="114">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1306,7 +1327,9 @@
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -1425,7 +1448,25 @@
       </c>
     </row>
     <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -1467,7 +1508,6 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:13">
-      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="H16" s="1"/>
@@ -2309,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2338,7 +2378,7 @@
         <v>15</v>
       </c>
       <c r="C2">
-        <v>4.5999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2354,13 +2394,13 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2368,10 +2408,10 @@
         <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2379,10 +2419,10 @@
         <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="C6">
-        <v>3.5</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2390,7 +2430,7 @@
         <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>3.5</v>
@@ -2401,18 +2441,18 @@
         <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -2426,7 +2466,7 @@
         <v>55</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2485,7 +2525,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C15" xr:uid="{BA28F66E-87F6-4624-831E-AD072F5E39A6}"/>
+  <autoFilter ref="A1:C15" xr:uid="{BA28F66E-87F6-4624-831E-AD072F5E39A6}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C15">
+      <sortCondition ref="A1:A15"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update job desc for USYD
</commit_message>
<xml_diff>
--- a/resume_data.xlsx
+++ b/resume_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\work project\vitae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4731A67-6594-4D04-8CFF-B3490053BF5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8761F5-5CA6-48C1-9007-7A4E815B6E25}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="94">
   <si>
     <t>section</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Assisted with the preparation of reconciliations of financial and operational data from different sources and provided recommendations to Finance Managers and Head of Schools</t>
   </si>
   <si>
-    <t>Assisted with providing budget and forecast for multiple stakeholders</t>
-  </si>
-  <si>
     <t>Data Analyst Intern</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
@@ -353,6 +350,12 @@
   <si>
     <t>Attended meetings with multiple project stakeholders including internal and external clients to gather and document detailed data requirements.</t>
     <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Designed, developed and maintained standardized budget/forecast models, tools and guidelines to improve the accuracy, consistency, timeliness and quality of budgeting and forecasting throughout the Faculties and these are continued to be used across the University faculties.</t>
+  </si>
+  <si>
+    <t>Performed variance analysis, trend analysis and sensitivity analysis on daily requests. Assisting Senior Financial Analyst in providing insightful analysis, to track and report financial and non-financial KPIs.</t>
   </si>
 </sst>
 </file>
@@ -1225,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1243,7 +1246,7 @@
     <col min="14" max="15" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1307,7 +1310,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="28.5">
+    <row r="3" spans="1:15" ht="28.5">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1333,7 +1336,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="28.5">
+    <row r="4" spans="1:15" ht="28.5">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1359,7 +1362,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="142.5">
+    <row r="5" spans="1:15" ht="142.5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1376,31 +1379,31 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="128.25">
+    </row>
+    <row r="6" spans="1:15" ht="171">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1417,25 +1420,30 @@
         <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="H6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="L6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="99.75">
+      <c r="N6"/>
+      <c r="O6"/>
+    </row>
+    <row r="7" spans="1:15" ht="99.75">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1443,7 +1451,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -1452,28 +1460,28 @@
         <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="185.25">
+    </row>
+    <row r="8" spans="1:15" ht="185.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1481,128 +1489,128 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="H8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="28.5">
+    </row>
+    <row r="9" spans="1:15" ht="28.5">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="42.75">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="42.75">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="J10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:15">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:15">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:15">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="H16" s="5"/>
@@ -2467,7 +2475,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -2478,7 +2486,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -2489,7 +2497,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -2500,7 +2508,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -2511,10 +2519,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6">
         <v>4.9000000000000004</v>
@@ -2522,7 +2530,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -2533,10 +2541,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
         <v>66</v>
-      </c>
-      <c r="B8" t="s">
-        <v>67</v>
       </c>
       <c r="C8">
         <v>3.5</v>
@@ -2544,10 +2552,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -2555,10 +2563,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -2566,10 +2574,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11">
         <v>3.5</v>
@@ -2577,10 +2585,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -2588,10 +2596,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -2599,10 +2607,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -2610,10 +2618,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
         <v>55</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
       </c>
       <c r="C15">
         <v>3.5</v>
@@ -2621,10 +2629,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
         <v>74</v>
-      </c>
-      <c r="B16" t="s">
-        <v>75</v>
       </c>
       <c r="C16">
         <v>2.5</v>

</xml_diff>